<commit_message>
Code refactoring and new functionalities added
</commit_message>
<xml_diff>
--- a/gs.xlsx
+++ b/gs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>Thales Alenia Space Center Madrid</t>
   </si>
@@ -74,9 +74,6 @@
     <t>[0;0;1]</t>
   </si>
   <si>
-    <t>Antenna</t>
-  </si>
-  <si>
     <t>Latitude (degrees)</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>Transmitter Power (dBW)</t>
+  </si>
+  <si>
+    <t>Antenna Type</t>
+  </si>
+  <si>
+    <t>Antenna Beam Aperture (degrees)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H7"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +529,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>40.591695366716998</v>
@@ -567,7 +570,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>-3.7090422957437199</v>
@@ -608,7 +611,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
@@ -649,7 +652,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -684,7 +687,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
@@ -719,7 +722,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -754,7 +757,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -795,7 +798,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -836,7 +839,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
@@ -877,7 +880,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -918,206 +921,247 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="C13" s="3">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="D13" s="3">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="F13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="G13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="H13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="I13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="J13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="K13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="L13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="M13" s="3">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="C14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="D14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="E14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="F14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="G14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="H14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="I14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="J14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="K14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="L14" s="4">
-        <v>14000000000</v>
-      </c>
-      <c r="M14" s="4">
-        <v>14000000000</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3">
+        <v>5</v>
+      </c>
+      <c r="J14" s="3">
+        <v>5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>5</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3">
-        <v>10</v>
-      </c>
-      <c r="E15" s="3">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3">
-        <v>10</v>
-      </c>
-      <c r="G15" s="3">
-        <v>10</v>
-      </c>
-      <c r="H15" s="3">
-        <v>10</v>
-      </c>
-      <c r="I15" s="3">
-        <v>10</v>
-      </c>
-      <c r="J15" s="3">
-        <v>10</v>
-      </c>
-      <c r="K15" s="3">
-        <v>10</v>
-      </c>
-      <c r="L15" s="3">
-        <v>10</v>
-      </c>
-      <c r="M15" s="3">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1400000000</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1400000000</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L16" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M16" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3">
+        <v>12</v>
+      </c>
+      <c r="H17" s="3">
+        <v>12</v>
+      </c>
+      <c r="I17" s="3">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3">
+        <v>12</v>
+      </c>
+      <c r="K17" s="3">
+        <v>12</v>
+      </c>
+      <c r="L17" s="3">
+        <v>12</v>
+      </c>
+      <c r="M17" s="3">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GUI updated and mission plan format modified
</commit_message>
<xml_diff>
--- a/gs.xlsx
+++ b/gs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TFG Aero\codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\mission_planning_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,9 +89,6 @@
     <t>Gimbal Mounting Angles (degrees)</t>
   </si>
   <si>
-    <t>Receiver Mounting Location (degrees)</t>
-  </si>
-  <si>
     <t>Receiver Gain to Noise Temperature ratio (dB)</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Antenna Beam Aperture (degrees)</t>
+  </si>
+  <si>
+    <t>RF equipment Mounting Location (meters)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
@@ -757,7 +757,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -921,48 +921,48 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>70</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4">
         <v>1400000000</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3">
         <v>10</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3">
         <v>12</v>

</xml_diff>

<commit_message>
Program updated and refactoring v1.2
</commit_message>
<xml_diff>
--- a/gs.xlsx
+++ b/gs.xlsx
@@ -59,9 +59,6 @@
     <t>AWS Singapore</t>
   </si>
   <si>
-    <t>ASW Sydney</t>
-  </si>
-  <si>
     <t>GS Name</t>
   </si>
   <si>
@@ -122,7 +119,10 @@
     <t>Antenna Beam Aperture (degrees)</t>
   </si>
   <si>
-    <t>RF equipment Mounting Location (meters)</t>
+    <t>AWS Sydney</t>
+  </si>
+  <si>
+    <t>RF equipment Mounting Angles (degrees)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -524,12 +524,12 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>40.591695366716998</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>-3.7090422957437199</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
@@ -652,72 +652,72 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -726,38 +726,38 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -921,48 +921,48 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3">
         <v>70</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4">
         <v>1400000000</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3">
         <v>10</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3">
         <v>12</v>

</xml_diff>